<commit_message>
12/02/2015 : Ajout onglet données
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developpement\Projects\ConseilApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Données" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -299,12 +304,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -346,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,7 +389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -595,11 +603,11 @@
   </sheetPr>
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -921,9 +929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -935,7 +943,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Création des scripts de données pour les styles et quelques paramètres
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="1" r:id="rId1"/>
     <sheet name="Données" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
   <si>
     <t>Conseil</t>
   </si>
@@ -180,13 +180,145 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>insert into style (Nom) values ('Rock')</t>
+  </si>
+  <si>
+    <t>insert into style (Nom) values ('Classique')</t>
+  </si>
+  <si>
+    <t>insert into style (Nom) values ('Urbain')</t>
+  </si>
+  <si>
+    <t>insert into style (Nom) values ('Sport')</t>
+  </si>
+  <si>
+    <t>insert into style (Nom) values ('Retro')</t>
+  </si>
+  <si>
+    <t>insert into style (Nom) values ('Traditionnel')</t>
+  </si>
+  <si>
+    <t>Type statut personne (historique)</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (1,'PersonneStatus','Abonne','Personne abonnée')</t>
+  </si>
+  <si>
+    <t>Type de photo</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (1,'PersonneStatus','EnAttente','Personne en attente')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (1,'PersonneStatus','Conseiller','Personne conseiller')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (2,'PhotoType','Habille','Photo de personne habillé')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (2,'PhotoType','Vetement','Photo de vêtement')</t>
+  </si>
+  <si>
+    <t>Type de message</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (3,'MessageType','Message','Message simple')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (3,'MessageType','Notification','Notification')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (3,'MessageType','Information','Information')</t>
+  </si>
+  <si>
+    <t>Type statut demande</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AttenteDemandeur','AttenteDemandeur')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AttenteConseiller','AttenteConseiller')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','Accepte','Accepte')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','RefusDemandeur','RefusDemandeur')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','RefusConseiller','RefusConseiller')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AnnulAdmin','AnnulAdmin')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','Termine','Termine')</t>
+  </si>
+  <si>
+    <t>Type de vêtement</t>
+  </si>
+  <si>
+    <t>VetementType</t>
+  </si>
+  <si>
+    <t>Tete</t>
+  </si>
+  <si>
+    <t>Type compteur</t>
+  </si>
+  <si>
+    <t>CompteurType</t>
+  </si>
+  <si>
+    <t>Abonne</t>
+  </si>
+  <si>
+    <t>Conseiller</t>
+  </si>
+  <si>
+    <t>Type de notification</t>
+  </si>
+  <si>
+    <t>NotifType</t>
+  </si>
+  <si>
+    <t>PropositionAccept,</t>
+  </si>
+  <si>
+    <t>PropositionReject,</t>
+  </si>
+  <si>
+    <t>PropositionCreation</t>
+  </si>
+  <si>
+    <t>DemandAccept,</t>
+  </si>
+  <si>
+    <t>DemandReject</t>
+  </si>
+  <si>
+    <t>Buste,</t>
+  </si>
+  <si>
+    <t>Jambe,</t>
+  </si>
+  <si>
+    <t>Pied,</t>
+  </si>
+  <si>
+    <t>Accessoire</t>
+  </si>
+  <si>
+    <t>DemandCreation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +344,15 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -284,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -294,6 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +746,7 @@
   <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="J15" sqref="J15:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,13 +1069,280 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
15/02/2015 : Reconnexion avec la base de données
Problème avec l'ajout d'enregistrement dans la table Personne (erreur
avec IDENTITY de la clé primaire...)
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -5,23 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developpement\Projects\ConseilApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\ConseilApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="12590" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
     <sheet name="Données" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Identifiants de test" sheetId="3" r:id="rId3"/>
+    <sheet name="Script divers" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Conseil</t>
   </si>
@@ -236,82 +238,106 @@
     <t>Type statut demande</t>
   </si>
   <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AttenteDemandeur','AttenteDemandeur')</t>
-  </si>
-  <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AttenteConseiller','AttenteConseiller')</t>
-  </si>
-  <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','Accepte','Accepte')</t>
-  </si>
-  <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','RefusDemandeur','RefusDemandeur')</t>
-  </si>
-  <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','RefusConseiller','RefusConseiller')</t>
-  </si>
-  <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AnnulAdmin','AnnulAdmin')</t>
-  </si>
-  <si>
-    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','Termine','Termine')</t>
-  </si>
-  <si>
     <t>Type de vêtement</t>
   </si>
   <si>
     <t>VetementType</t>
   </si>
   <si>
-    <t>Tete</t>
-  </si>
-  <si>
     <t>Type compteur</t>
   </si>
   <si>
     <t>CompteurType</t>
   </si>
   <si>
-    <t>Abonne</t>
-  </si>
-  <si>
-    <t>Conseiller</t>
-  </si>
-  <si>
     <t>Type de notification</t>
   </si>
   <si>
     <t>NotifType</t>
   </si>
   <si>
-    <t>PropositionAccept,</t>
-  </si>
-  <si>
-    <t>PropositionReject,</t>
-  </si>
-  <si>
-    <t>PropositionCreation</t>
-  </si>
-  <si>
-    <t>DemandAccept,</t>
-  </si>
-  <si>
-    <t>DemandReject</t>
-  </si>
-  <si>
-    <t>Buste,</t>
-  </si>
-  <si>
-    <t>Jambe,</t>
-  </si>
-  <si>
-    <t>Pied,</t>
-  </si>
-  <si>
-    <t>Accessoire</t>
-  </si>
-  <si>
-    <t>DemandCreation</t>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (5,'VetementType','Buste','Buste')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (5,'VetementType','Tete','Tête')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (5,'VetementType','Jambe','Jambe')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (5,'VetementType','Pied','Pied')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (5,'VetementType','Accessoire','Accessoire')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (5,'VetementType','Main','Main')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (6,'CompteurType','Abonne','Abonné')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (6,'CompteurType','Conseiller','Conseiller')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (7,'NotifType','PropositionAccept','Proposition acceptée')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (7,'NotifType','PropositionReject','Proposition rejetée')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (7,'NotifType','DemandeCreation','Demander une aide')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (7,'NotifType','PropositionCreation','Proposer une aide')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (7,'NotifType','DemandeAccept','Demande acceptée')</t>
+  </si>
+  <si>
+    <t>insert into typeparam (TypeId, TypeLib, ParamCode, ParamLib) values (7,'NotifType','DemandeReject','Demande rejetée')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AttenteDemandeur','Proposition en attente réponse demandeur')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AttenteConseiller','Demande en attente réponse conseiller')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','Accepte','Demande ou proposition acceptée')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','RefusDemandeur','Proposition refusée par demandeur')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','RefusConseiller','Demande refusée par conseiller')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','AnnulAdmin','Demande ou proposition annulée par administrateur')</t>
+  </si>
+  <si>
+    <t>insert into dbo.TypeParam (TypeId, TypeLib, ParamCode, ParamLib) values (4,'DemandeStatus','Termine','Demande ou proposition terminée')</t>
+  </si>
+  <si>
+    <t>userA</t>
+  </si>
+  <si>
+    <t>mdpmdpA</t>
+  </si>
+  <si>
+    <t>DBCC CHECKIDENT ('dbo.UserProfile');</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>DBCC CHECKIDENT ('dbo.webpages_Membership');</t>
+  </si>
+  <si>
+    <t>USE ModeConseil</t>
+  </si>
+  <si>
+    <t>DBCC CHECKIDENT ('Personne');</t>
   </si>
 </sst>
 </file>
@@ -749,24 +775,24 @@
       <selection activeCell="J15" sqref="J15:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -791,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -811,7 +837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -831,7 +857,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -848,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -865,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -882,7 +908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -896,7 +922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -904,7 +930,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -912,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -920,13 +946,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -951,7 +977,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
@@ -971,7 +997,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
@@ -991,7 +1017,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1028,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1018,8 +1044,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
@@ -1027,7 +1053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
@@ -1035,7 +1061,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1043,7 +1069,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1051,12 +1077,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="D27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1069,275 +1095,280 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E60"/>
+  <dimension ref="B1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="E43" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="E51" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="E55" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1348,12 +1379,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17/02/2015 : PB de base de données résolue
Rejoué le script de création de la base (remanié) qui se trouve dans le
fichier Excel.
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\ConseilApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developpement\Projects\ConseilApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="12590" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
     <sheet name="Données" sheetId="2" r:id="rId2"/>
     <sheet name="Identifiants de test" sheetId="3" r:id="rId3"/>
     <sheet name="Script divers" sheetId="4" r:id="rId4"/>
+    <sheet name="Creation de la base" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="412">
   <si>
     <t>Conseil</t>
   </si>
@@ -338,13 +338,934 @@
   </si>
   <si>
     <t>DBCC CHECKIDENT ('Personne');</t>
+  </si>
+  <si>
+    <t>-- --------------------------------------------------</t>
+  </si>
+  <si>
+    <t>-- Entity Designer DDL Script for SQL Server 2005, 2008, 2012 and Azure</t>
+  </si>
+  <si>
+    <t>-- Date Created: 02/16/2015 23:15:33</t>
+  </si>
+  <si>
+    <t>SET QUOTED_IDENTIFIER OFF;</t>
+  </si>
+  <si>
+    <t>USE [ModeConseil];</t>
+  </si>
+  <si>
+    <t>IF SCHEMA_ID(N'dbo') IS NULL EXECUTE(N'CREATE SCHEMA [dbo]');</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Conseil_PersonneConseille]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Conseil] DROP CONSTRAINT [FK_Conseil_PersonneConseille];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Conseil_PersonneDemande]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Conseil] DROP CONSTRAINT [FK_Conseil_PersonneDemande];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Conseil_Style]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Conseil] DROP CONSTRAINT [FK_Conseil_Style];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Conseil_TypeParam]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Conseil] DROP CONSTRAINT [FK_Conseil_TypeParam];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Habillage_Conseil]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Habillage] DROP CONSTRAINT [FK_Habillage_Conseil];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Notification_Conseil]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Notification] DROP CONSTRAINT [FK_Notification_Conseil];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Notification_Personne]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Notification] DROP CONSTRAINT [FK_Notification_Personne];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Notification_TypeParam]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Notification] DROP CONSTRAINT [FK_Notification_TypeParam];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Photo_Personne]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Photo] DROP CONSTRAINT [FK_Photo_Personne];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Photo_TypeParam]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Photo] DROP CONSTRAINT [FK_Photo_TypeParam];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Photo_Vetement]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Photo] DROP CONSTRAINT [FK_Photo_Vetement];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_PhotoHabillage_Habillage]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[PhotoHabillage] DROP CONSTRAINT [FK_PhotoHabillage_Habillage];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_PhotoHabillage_Photo]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[PhotoHabillage] DROP CONSTRAINT [FK_PhotoHabillage_Photo];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_PhotoStyle_Photo]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[PhotoStyle] DROP CONSTRAINT [FK_PhotoStyle_Photo];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_PhotoStyle_Style]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[PhotoStyle] DROP CONSTRAINT [FK_PhotoStyle_Style];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_StatutHistorique_Personne]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[StatutHistorique] DROP CONSTRAINT [FK_StatutHistorique_Personne];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_StatutHistorique_Style]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[StatutHistorique] DROP CONSTRAINT [FK_StatutHistorique_Style];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_StatutHistorique_TypeParam]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[StatutHistorique] DROP CONSTRAINT [FK_StatutHistorique_TypeParam];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_SuiviTelecharge_Personne]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[SuiviTelecharge] DROP CONSTRAINT [FK_SuiviTelecharge_Personne];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[FK_Vetement_TypeParam]', 'F') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ALTER TABLE [dbo].[Vetement] DROP CONSTRAINT [FK_Vetement_TypeParam];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Conseil]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Conseil];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Habillage]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Habillage];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Notification]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Notification];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Personne]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Personne];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Photo]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Photo];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[PhotoHabillage]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[PhotoHabillage];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[PhotoStyle]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[PhotoStyle];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[StatutHistorique]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[StatutHistorique];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Style]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Style];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[SuiviTelecharge]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[SuiviTelecharge];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[TypeParam]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[TypeParam];</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[Vetement]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[Vetement];</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Conseils'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Id] int IDENTITY(1,1) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DateCreation] datetime  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DateLimite] datetime  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DateAccepte] datetime  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DateRefuse] datetime  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DemandeurId] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ConseillerId] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [StyleId] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [TypeId] int  NOT NULL</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Habillages'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Commentaire] varchar(500)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Note] smallint  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ConseilId] int  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Notifications'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Message] varchar(500)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [TypeId] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [PersonneId] int  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ConseilId] int  NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Personnes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Id] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [FBCode] varchar(10)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Nom] varchar(100)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Prenom] varchar(150)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Pseudo] varchar(50)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Email] varchar(500)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Genre] char(1)  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [AfficheInfo] bit  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [EnvoiEmail] bit  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [MotPasse] nvarchar(500)  NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Photos'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Url] varchar(250)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [VetementId] int  NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [PersonneId] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [DateTelecharge] datetime  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'StatutHistoriques'</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Styles'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Nom] varchar(200)  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'SuiviTelecharges'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jour] datetime  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Compteur] tinyint  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'TypeParams'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [TypeId] tinyint  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [TypeLib] varchar(50)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ParamCode] varchar(25)  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [ParamLib] varchar(200)  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'UserProfiles'</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[UserProfiles] (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [UserId] int IDENTITY(1,1) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [UserName] nvarchar(56)  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'Vetements'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Nom] varchar(200)  NOT NULL,</t>
+  </si>
+  <si>
+    <t>-- Creating table 'PhotoHabillage'</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[PhotoHabillage] (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Habillages_Id] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Photos_Id] int  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating table 'PhotoStyle'</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[PhotoStyle] (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Photos_Id] int  NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Styles_Id] int  NOT NULL</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Conseils'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Conseils]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PRIMARY KEY CLUSTERED ([Id] ASC);</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Habillages'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Habillages]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Notifications'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Notifications]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Personnes'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Personnes]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Photos'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Photos]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'StatutHistoriques'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_StatutHistoriques]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Styles'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Styles]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Jour], [PersonneId], [Compteur] in table 'SuiviTelecharges'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_SuiviTelecharges]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PRIMARY KEY CLUSTERED ([Jour], [PersonneId], [Compteur] ASC);</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'TypeParams'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_TypeParams]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [UserId] in table 'UserProfiles'</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[UserProfiles]</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_UserProfiles]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PRIMARY KEY CLUSTERED ([UserId] ASC);</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Id] in table 'Vetements'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_Vetements]</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Habillages_Id], [Photos_Id] in table 'PhotoHabillage'</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[PhotoHabillage]</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_PhotoHabillage]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PRIMARY KEY CLUSTERED ([Habillages_Id], [Photos_Id] ASC);</t>
+  </si>
+  <si>
+    <t>-- Creating primary key on [Photos_Id], [Styles_Id] in table 'PhotoStyle'</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[PhotoStyle]</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [PK_PhotoStyle]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PRIMARY KEY CLUSTERED ([Photos_Id], [Styles_Id] ASC);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [ConseillerId] in table 'Conseils'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Conseil_PersonneConseille]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([ConseillerId])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ([Id])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ON DELETE NO ACTION ON UPDATE NO ACTION;</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Conseil_PersonneConseille'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Conseil_PersonneConseille]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([ConseillerId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [DemandeurId] in table 'Conseils'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Conseil_PersonneDemande]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([DemandeurId])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Conseil_PersonneDemande'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Conseil_PersonneDemande]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([DemandeurId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [StyleId] in table 'Conseils'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Conseil_Style]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([StyleId])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Conseil_Style'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Conseil_Style]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([StyleId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [TypeId] in table 'Conseils'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Conseil_TypeParam]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([TypeId])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Conseil_TypeParam'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Conseil_TypeParam]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([TypeId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [ConseilId] in table 'Habillages'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Habillage_Conseil]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([ConseilId])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Habillage_Conseil'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Habillage_Conseil]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([ConseilId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [ConseilId] in table 'Notifications'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Notification_Conseil]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Notification_Conseil'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Notification_Conseil]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [PersonneId] in table 'Notifications'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Notification_Personne]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([PersonneId])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Notification_Personne'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Notification_Personne]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([PersonneId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [TypeId] in table 'Notifications'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Notification_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Notification_TypeParam'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Notification_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [PersonneId] in table 'Photos'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Photo_Personne]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Photo_Personne'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Photo_Personne]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [PersonneId] in table 'StatutHistoriques'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_StatutHistorique_Personne]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_StatutHistorique_Personne'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_StatutHistorique_Personne]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [PersonneId] in table 'SuiviTelecharges'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_SuiviTelecharge_Personne]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_SuiviTelecharge_Personne'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_SuiviTelecharge_Personne]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [TypeId] in table 'Photos'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Photo_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Photo_TypeParam'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Photo_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [VetementId] in table 'Photos'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Photo_Vetement]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([VetementId])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Photo_Vetement'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Photo_Vetement]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([VetementId]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [StyleId] in table 'StatutHistoriques'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_StatutHistorique_Style]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_StatutHistorique_Style'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_StatutHistorique_Style]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [TypeId] in table 'StatutHistoriques'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_StatutHistorique_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_StatutHistorique_TypeParam'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_StatutHistorique_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [TypeId] in table 'Vetements'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_Vetement_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_Vetement_TypeParam'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_Vetement_TypeParam]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [Habillages_Id] in table 'PhotoHabillage'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_PhotoHabillage_Habillage]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([Habillages_Id])</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [Photos_Id] in table 'PhotoHabillage'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_PhotoHabillage_Photo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([Photos_Id])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_PhotoHabillage_Photo'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_PhotoHabillage_Photo]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[PhotoHabillage]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([Photos_Id]);</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [Photos_Id] in table 'PhotoStyle'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_PhotoStyle_Photo]</t>
+  </si>
+  <si>
+    <t>-- Creating foreign key on [Styles_Id] in table 'PhotoStyle'</t>
+  </si>
+  <si>
+    <t>ADD CONSTRAINT [FK_PhotoStyle_Style]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    FOREIGN KEY ([Styles_Id])</t>
+  </si>
+  <si>
+    <t>-- Creating non-clustered index for FOREIGN KEY 'FK_PhotoStyle_Style'</t>
+  </si>
+  <si>
+    <t>CREATE INDEX [IX_FK_PhotoStyle_Style]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[PhotoStyle]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([Styles_Id]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Generated from EDMX file:('C'):\Developpement\Projects\ConseilApp\ConseilDAL\DataModel.edmx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Dropping existing FOREIGN KEY constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Dropping existing tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Creating all tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Creating all FOREIGN KEY constraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Script has ended</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Creating all PRIMARY KEY constraints</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Conseil] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Conseil]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[Conseil]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[Conseil]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Habillage] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Habillage]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[Habillage]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[Habillage]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Notification] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Notification]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[Notification]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Personne] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Personne]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[Personne]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Photo] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Photo]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[Photo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[Photo]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[StatutHistorique] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[StatutHistorique]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[StatutHistorique]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Style] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Style]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[Style]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[SuiviTelecharge] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[SuiviTelecharge]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[SuiviTelecharge]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[TypeParam] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[TypeParam]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[TypeParam]</t>
+  </si>
+  <si>
+    <t>CREATE TABLE [dbo].[Vetement] (</t>
+  </si>
+  <si>
+    <t>ALTER TABLE [dbo].[Vetement]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES [dbo].[Vetement]</t>
+  </si>
+  <si>
+    <t>ON [dbo].[Vetement]</t>
+  </si>
+  <si>
+    <t>IF OBJECT_ID(N'[dbo].[UserProfiles]', 'U') IS NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    DROP TABLE [dbo].[UserProfiles];</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +1302,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,7 +1379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -462,6 +1390,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,24 +1704,24 @@
       <selection activeCell="J15" sqref="J15:J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -817,7 +1746,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -837,7 +1766,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -857,7 +1786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -874,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -891,7 +1820,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -908,7 +1837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -922,7 +1851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -930,7 +1859,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -938,7 +1867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -946,13 +1875,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -977,7 +1906,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
@@ -997,7 +1926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
@@ -1017,7 +1946,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>8</v>
       </c>
@@ -1028,7 +1957,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1965,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1044,8 +1973,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
@@ -1053,7 +1982,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
@@ -1061,7 +1990,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1069,7 +1998,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1077,12 +2006,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1097,187 +2026,187 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>71</v>
       </c>
@@ -1285,37 +2214,37 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>73</v>
       </c>
@@ -1323,17 +2252,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>75</v>
       </c>
@@ -1341,32 +2270,32 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>88</v>
       </c>
@@ -1385,9 +2314,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1404,48 +2333,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1453,4 +2382,2800 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A630"/>
+  <sheetViews>
+    <sheetView topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="A340" sqref="A340:A626"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="626" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="628" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="629" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="630" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revu de la gestion du menu
modification de la création du menu
RAF : pouvoir maj le menu lorsque l'on change de style dans la
dropdown... Piste avec la recharge de la page sur laquelle on se trouve
??!!
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="12590" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Identifiants de test" sheetId="3" r:id="rId3"/>
     <sheet name="Script divers" sheetId="4" r:id="rId4"/>
     <sheet name="Creation de la base" sheetId="5" r:id="rId5"/>
+    <sheet name="TODO Liste" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="456">
   <si>
     <t>Conseil</t>
   </si>
@@ -1334,13 +1335,70 @@
   </si>
   <si>
     <t xml:space="preserve">    ([PhotoId]);</t>
+  </si>
+  <si>
+    <t>Revoir le style général du site</t>
+  </si>
+  <si>
+    <t>créer une vue pour le détail des deux tableaux :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - attenteConseil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - proposeAide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - apteConseil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - solliciteAide</t>
+  </si>
+  <si>
+    <t>Page "Mes propositions" modifier la présentation des tableaux (sous forme de gridTemplate)</t>
+  </si>
+  <si>
+    <t>Page "Mes demandes" modifier la présentation des tableaux (sous forme de gridTemplate)</t>
+  </si>
+  <si>
+    <t>Implémenter les notifications dans la BLL</t>
+  </si>
+  <si>
+    <t>Implémenter les vues d'interaction (accept/refuse) pour les demandes et les propositions</t>
+  </si>
+  <si>
+    <t>Implémenter la vue modal qui permet de choisir un abonné dans une vue partielle avec un modèle générique au 4 traitements</t>
+  </si>
+  <si>
+    <t>Implémente l'affichage des menus "Demandes" et "Propositions" en fonction du statut de la personne connectée</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ==&gt; il faut implémenter un traitement pour récupérer le statut le l'utilisateur connecté en fonction du style sélectionné dans la liste sous le menu. Tout cela avant de renseigner "Viewbag.TypeAbonne"</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com/components/#input-groups-buttons-dropdowns</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com/components/#badges</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com/components/#jumbotron</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com/components/#breadcrumbs</t>
+  </si>
+  <si>
+    <t>dans le footer</t>
+  </si>
+  <si>
+    <t>Mise en place d'une nouvelle gestion du menu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1384,6 +1442,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1451,10 +1524,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1470,8 +1544,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1783,24 +1861,24 @@
       <selection activeCell="B23" sqref="B23:B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1825,7 +1903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1845,7 +1923,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +1943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1882,7 +1960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1899,7 +1977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1916,7 +1994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1930,7 +2008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1938,7 +2016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1946,7 +2024,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1954,13 +2032,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -1985,7 +2063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
@@ -2005,7 +2083,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
@@ -2025,7 +2103,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2114,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2122,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="5" t="s">
         <v>9</v>
       </c>
@@ -2052,8 +2130,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
@@ -2061,7 +2139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
@@ -2069,7 +2147,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -2077,7 +2155,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
@@ -2085,12 +2163,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="6" t="s">
         <v>52</v>
       </c>
@@ -2109,183 +2187,183 @@
       <selection activeCell="L51" sqref="L51:L61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>71</v>
       </c>
@@ -2293,7 +2371,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>16</v>
       </c>
@@ -2301,7 +2379,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>17</v>
       </c>
@@ -2309,7 +2387,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>18</v>
       </c>
@@ -2317,7 +2395,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>19</v>
       </c>
@@ -2325,7 +2403,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>20</v>
       </c>
@@ -2333,7 +2411,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>21</v>
       </c>
@@ -2341,8 +2419,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="8" t="s">
         <v>47</v>
       </c>
@@ -2353,7 +2431,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2442,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C53" s="3" t="s">
         <v>19</v>
       </c>
@@ -2375,7 +2453,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
@@ -2386,7 +2464,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
         <v>401</v>
       </c>
@@ -2394,7 +2472,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>404</v>
       </c>
@@ -2402,7 +2480,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>402</v>
       </c>
@@ -2410,7 +2488,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>403</v>
       </c>
@@ -2418,7 +2496,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>405</v>
       </c>
@@ -2426,7 +2504,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>406</v>
       </c>
@@ -2434,7 +2512,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>407</v>
       </c>
@@ -2442,32 +2520,32 @@
         <v>423</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
         <v>73</v>
       </c>
@@ -2475,17 +2553,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
         <v>75</v>
       </c>
@@ -2493,32 +2571,32 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>88</v>
       </c>
@@ -2537,9 +2615,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2560,44 +2638,44 @@
       <selection activeCell="A5" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -2611,2791 +2689,2791 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.90625" style="11"/>
+    <col min="1" max="16384" width="10.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="11" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="11" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="11" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="11" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="11" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="11" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="11" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="11" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="11" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="11" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="11" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="11" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="11" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="11" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="11" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="11" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="11" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="11" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="11" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="11" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="11" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="11" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="11" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="11" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="11" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="11" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="11" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="11" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="11" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="11" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="11" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="11" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="11" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="11" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="12" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="12" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="12" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="11" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="11" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="11" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="11" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="11" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="11" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="11" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="11" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="11" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="11" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="11" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="11" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="11" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" s="11" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="11" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="11" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="11" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="11" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" s="11" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="11" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="11" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="11" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" s="11" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="11" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="11" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="11" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="11" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" s="11" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="11" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="11" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" s="11" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="11" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" s="11" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="11" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="11" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="11" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" s="11" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" s="11" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="11" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" s="11" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="11" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="11" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" s="11" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="11" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" s="11" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" s="11" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" s="11" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" s="11" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="11" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" s="11" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="11" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" s="11" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" s="11" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" s="11" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" s="11" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="11" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" s="11" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" s="11" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" s="11" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" s="11" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" s="11" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" s="11" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515" s="11" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" s="11" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A520" s="11" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A521" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" s="11" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" s="11" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" s="11" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" s="11" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" s="11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" s="11" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" s="11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" s="11" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" s="11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544" s="11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" s="11" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A557" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A559" s="11" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" s="11" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="561" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A561" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="562" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="563" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A563" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="565" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A565" s="11" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="566" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" s="11" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="567" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A567" s="11" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="568" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A568" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="569" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A569" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="570" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A570" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="571" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A571" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="572" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A572" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="574" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A574" s="11" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="575" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A575" s="11" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" s="11" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="577" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A577" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="578" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="580" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" s="11" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="581" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" s="11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="582" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A582" s="11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="583" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A583" s="11" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="584" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" s="11" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="585" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A585" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="586" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A586" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="587" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A587" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="589" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A589" s="11" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="590" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" s="11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="591" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A591" s="11" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="592" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A592" s="11" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="593" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A593" s="11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="594" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="595" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A595" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="596" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A596" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="598" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A598" s="11" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="599" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A599" s="11" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="600" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A600" s="11" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="601" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A601" s="11" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="602" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A602" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="604" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A604" s="11" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="605" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A605" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="606" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A606" s="11" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="607" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A607" s="11" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="608" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A608" s="11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A609" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A610" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A611" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="613" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A613" s="11" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="614" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A614" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="615" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A615" s="11" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="616" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A616" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="617" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A617" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="618" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A618" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="619" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A619" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="620" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A620" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="622" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A622" s="11" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A623" s="11" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="624" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="624" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A624" s="11" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="625" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="625" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A625" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="626" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="626" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A626" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="628" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="628" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A628" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="629" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="629" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A629" s="11" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="630" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="630" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A630" s="11" t="s">
         <v>105</v>
       </c>
@@ -5404,4 +5482,121 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="14" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="15" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>453</v>
+      </c>
+      <c r="I20" t="s">
+        <v>454</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D17" r:id="rId1" location="input-groups-buttons-dropdowns"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
03/03/2015 : Gestion du changement de style
Liste des styles redessinée et déplacée dans les pages Demandes et
Propositions. Gestion du rafraîchissement des tableaux (PartialView)
lorsque l'on change de style.
Revu de code avec l'analyseur de code intégré à VS.
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="458">
   <si>
     <t>Conseil</t>
   </si>
@@ -1392,6 +1392,12 @@
   </si>
   <si>
     <t>Mise en place d'une nouvelle gestion du menu</t>
+  </si>
+  <si>
+    <t>Régler le problème de la liste des styles dans la page des Upload pour les habillages</t>
+  </si>
+  <si>
+    <t>il faut afficher uniquement les styles pour lesquels la personne est conseiller !</t>
   </si>
 </sst>
 </file>
@@ -5486,10 +5492,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I20"/>
+  <dimension ref="C2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5569,27 +5575,37 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D17" s="15" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>453</v>
       </c>
       <c r="I20" t="s">
         <v>454</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="13" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
21/03/2015 : Concevoir / Visualiser
Préparation des couches d'acces aux données pour les pages de conception
et de visualisation des habillages
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\ConseilApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developpement\Projects\ConseilApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="474">
   <si>
     <t>Conseil</t>
   </si>
@@ -1398,6 +1398,54 @@
   </si>
   <si>
     <t>il faut afficher uniquement les styles pour lesquels la personne est conseiller !</t>
+  </si>
+  <si>
+    <t>Liste des conseils selon un ou des status ; un conseiller ou un demandeur ; un style</t>
+  </si>
+  <si>
+    <t>Liste des habillages pour un conseil</t>
+  </si>
+  <si>
+    <t>Liste des photos d'un habillage</t>
+  </si>
+  <si>
+    <t>Liste des types de vêtement</t>
+  </si>
+  <si>
+    <t>Envoi d'un message d'une personne à une autre</t>
+  </si>
+  <si>
+    <t>Envoi note et commentaire pour un habillage</t>
+  </si>
+  <si>
+    <t>Clôture un conseil</t>
+  </si>
+  <si>
+    <t>Envoi habillage et commentaire</t>
+  </si>
+  <si>
+    <t>Détails</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Vue</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Liste des photos d'une personne pour un type de vêtement (GetPicsByPersonVetementStyle)</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1516,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1481,8 +1529,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1529,12 +1583,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1553,6 +1739,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -5492,10 +5702,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I23"/>
+  <dimension ref="C2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,22 +5785,22 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D17" s="15" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>453</v>
       </c>
@@ -5598,17 +5808,200 @@
         <v>454</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D23" s="13" t="s">
         <v>457</v>
       </c>
     </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>470</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="24" t="s">
+        <v>458</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="27" t="s">
+        <v>459</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C29" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="30" t="s">
+        <v>472</v>
+      </c>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C30" s="27" t="s">
+        <v>461</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C31" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C32" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C33" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C34" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C35" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C26:I26"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D17" r:id="rId1" location="input-groups-buttons-dropdowns"/>
   </hyperlinks>

</xml_diff>

<commit_message>
24/03/2015 : Concevoir / Visualiser
Implémente les méthodes dans les couches Repository et BLL
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developpement\Projects\ConseilApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\ConseilApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="474">
   <si>
     <t>Conseil</t>
   </si>
@@ -1415,15 +1415,9 @@
     <t>Envoi d'un message d'une personne à une autre</t>
   </si>
   <si>
-    <t>Envoi note et commentaire pour un habillage</t>
-  </si>
-  <si>
     <t>Clôture un conseil</t>
   </si>
   <si>
-    <t>Envoi habillage et commentaire</t>
-  </si>
-  <si>
     <t>Détails</t>
   </si>
   <si>
@@ -1446,6 +1440,12 @@
   </si>
   <si>
     <t>Liste des photos d'une personne pour un type de vêtement (GetPicsByPersonVetementStyle)</t>
+  </si>
+  <si>
+    <t>Créer un habillage</t>
+  </si>
+  <si>
+    <t>Donner une note à l'habillage (modifier un habillage)</t>
   </si>
 </sst>
 </file>
@@ -1742,9 +1742,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1761,6 +1758,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2077,24 +2077,24 @@
       <selection activeCell="B23" sqref="B23:B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -2248,13 +2248,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="4" t="s">
         <v>8</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="5" t="s">
         <v>9</v>
       </c>
@@ -2346,8 +2346,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
@@ -2379,12 +2379,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D28" s="6" t="s">
         <v>52</v>
       </c>
@@ -2403,183 +2403,183 @@
       <selection activeCell="L51" sqref="L51:L61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
         <v>71</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
         <v>16</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>17</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>18</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>19</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>20</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>21</v>
       </c>
@@ -2635,8 +2635,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="8" t="s">
         <v>47</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C52" s="2" t="s">
         <v>1</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
         <v>19</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E55" t="s">
         <v>401</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E56" t="s">
         <v>404</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E57" t="s">
         <v>402</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E58" t="s">
         <v>403</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E59" t="s">
         <v>405</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
         <v>406</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E61" t="s">
         <v>407</v>
       </c>
@@ -2736,32 +2736,32 @@
         <v>423</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E62" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E63" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E66" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="9" t="s">
         <v>73</v>
       </c>
@@ -2769,17 +2769,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="9" t="s">
         <v>75</v>
       </c>
@@ -2787,32 +2787,32 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>88</v>
       </c>
@@ -2831,9 +2831,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -2854,44 +2854,44 @@
       <selection activeCell="A5" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -2909,2787 +2909,2787 @@
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.85546875" style="11"/>
+    <col min="1" max="16384" width="10.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="11" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="11" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="11" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="11" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="11" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="11" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="11" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="11" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="11" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="11" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" s="11" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="11" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="11" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="11" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="11" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="11" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="11" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="11" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="11" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="11" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="11" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" s="11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="11" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="11" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" s="11" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="11" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="11" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="11" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" s="12" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="12" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="12" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="11" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="11" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" s="11" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="11" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" s="11" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="11" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" s="11" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="11" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="11" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="11" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" s="11" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" s="11" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" s="11" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="11" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" s="11" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" s="11" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="11" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="11" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="11" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" s="11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="11" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="11" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="11" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="11" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" s="11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" s="11" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" s="12" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" s="12" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" s="12" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" s="12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" s="11" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" s="11" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" s="11" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" s="11" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" s="11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" s="11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" s="11" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" s="11" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" s="11" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" s="11" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" s="11" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" s="11" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" s="11" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A347" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A349" s="11" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A350" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" s="11" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" s="11" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" s="11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" s="11" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" s="11" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A372" s="11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A375" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A376" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A377" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A379" s="11" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A380" s="11" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A381" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A382" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A383" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A385" s="11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A386" s="11" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A387" s="11" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A390" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A391" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A392" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" s="11" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A395" s="11" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A396" s="11" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" s="11" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A401" s="11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A402" s="11" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" s="11" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" s="11" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A406" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" s="11" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A410" s="11" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A411" s="11" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A412" s="11" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A413" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A415" s="11" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A416" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A417" s="11" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A418" s="11" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A419" s="11" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A420" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A421" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A422" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A424" s="11" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A425" s="11" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A426" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A427" s="11" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A428" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A430" s="11" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A431" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A432" s="11" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A433" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A434" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A435" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A436" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A437" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A439" s="11" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A440" s="11" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A441" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A442" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A443" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="11" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A446" s="11" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="11" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A448" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A449" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A450" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A451" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A452" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A454" s="11" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A455" s="11" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A456" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A457" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A458" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A460" s="11" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A461" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A462" s="11" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A463" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A464" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A465" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A466" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A467" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A469" s="11" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A470" s="11" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A471" s="11" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A472" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A473" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A475" s="11" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A476" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A477" s="11" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A478" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A479" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A480" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A481" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A482" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A484" s="11" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A485" s="11" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A486" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A487" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A488" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A490" s="11" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A491" s="11" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A492" s="11" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A493" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A494" s="11" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A495" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A496" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A497" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A499" s="11" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A500" s="11" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A501" s="11" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A502" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A503" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A505" s="11" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A506" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A507" s="11" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A508" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A509" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A510" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A511" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A512" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A514" s="11" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A515" s="11" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A516" s="11" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A517" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A518" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A520" s="11" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A521" s="11" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A522" s="11" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A523" s="11" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A524" s="11" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A525" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A526" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A527" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A529" s="11" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A530" s="11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A531" s="11" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532" s="11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A533" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A535" s="11" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A536" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A537" s="11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A538" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A539" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A540" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A541" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A542" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A544" s="11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A545" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A546" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A547" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A548" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A550" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A551" s="11" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A552" s="11" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A553" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A554" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A555" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A556" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A557" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A559" s="11" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A560" s="11" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A561" s="11" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A562" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A563" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A565" s="11" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A566" s="11" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A567" s="11" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A568" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A569" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A570" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A571" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A572" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A574" s="11" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A575" s="11" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A576" s="11" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A577" s="11" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A578" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A580" s="11" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A581" s="11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A582" s="11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A583" s="11" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A584" s="11" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A585" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A586" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A587" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A589" s="11" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A590" s="11" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A591" s="11" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A592" s="11" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A593" s="11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A594" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A595" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A596" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A598" s="11" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A599" s="11" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A600" s="11" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A601" s="11" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A602" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A604" s="11" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A605" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A606" s="11" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A607" s="11" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A608" s="11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A609" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A610" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A611" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A613" s="11" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A614" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A615" s="11" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A616" s="11" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A617" s="11" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A618" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A619" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A620" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A622" s="11" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A623" s="11" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="624" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A624" s="11" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="625" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A625" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="626" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A626" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="628" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A628" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="629" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A629" s="11" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="630" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A630" s="11" t="s">
         <v>105</v>
       </c>
@@ -5704,103 +5704,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="13" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="14" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D17" s="15" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>453</v>
       </c>
@@ -5808,195 +5808,221 @@
         <v>454</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
       <c r="D23" s="13" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="17" t="s">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C26" s="31" t="s">
+        <v>464</v>
+      </c>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="16" t="s">
+        <v>465</v>
+      </c>
+      <c r="K26" s="16" t="s">
         <v>466</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="16" t="s">
+      <c r="L26" s="16" t="s">
         <v>467</v>
       </c>
-      <c r="K26" s="16" t="s">
+      <c r="M26" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="L26" s="16" t="s">
+      <c r="N26" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="M26" s="16" t="s">
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C27" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="29" t="s">
         <v>470</v>
       </c>
-      <c r="N26" s="16" t="s">
+      <c r="K27" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C28" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C29" s="24" t="s">
+        <v>460</v>
+      </c>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C30" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C31" s="24" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C27" s="24" t="s">
-        <v>458</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="30" t="s">
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="K31" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C32" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C33" s="24" t="s">
+        <v>473</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="K33" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C34" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="K34" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C35" s="25" t="s">
         <v>472</v>
       </c>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="27" t="s">
-        <v>459</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="30" t="s">
-        <v>472</v>
-      </c>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="25" t="s">
-        <v>460</v>
-      </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="30" t="s">
-        <v>472</v>
-      </c>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C30" s="27" t="s">
-        <v>461</v>
-      </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="31" t="s">
-        <v>472</v>
-      </c>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C31" s="25" t="s">
-        <v>473</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="31" t="s">
-        <v>472</v>
-      </c>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C32" s="27" t="s">
-        <v>462</v>
-      </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-    </row>
-    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C33" s="25" t="s">
-        <v>463</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-    </row>
-    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="27" t="s">
-        <v>464</v>
-      </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-    </row>
-    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="26" t="s">
-        <v>465</v>
-      </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="K35" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
29/03/2015 : Concevoir / Visualiser
Revu d'une méthode dans le repository Conseil.
Prépare le Builder pour les habillage.
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="480">
   <si>
     <t>Conseil</t>
   </si>
@@ -1446,6 +1446,24 @@
   </si>
   <si>
     <t>Donner une note à l'habillage (modifier un habillage)</t>
+  </si>
+  <si>
+    <t>Etude des modèles de données pour les vues :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - liste des conseillers </t>
+  </si>
+  <si>
+    <t>Visualiser les habillages :</t>
+  </si>
+  <si>
+    <t>Personne.Id</t>
+  </si>
+  <si>
+    <t>Personne.Pseudo</t>
+  </si>
+  <si>
+    <t>Conseil.DateCreation</t>
   </si>
 </sst>
 </file>
@@ -5702,10 +5720,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:N35"/>
+  <dimension ref="C2:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6023,6 +6041,36 @@
       <c r="L35" s="29"/>
       <c r="M35" s="29"/>
       <c r="N35" s="29"/>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>479</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>